<commit_message>
[Update Edit Customer] - Tab Job Data
</commit_message>
<xml_diff>
--- a/Data Files/LOS_EditCustomer_TestData.xlsx
+++ b/Data Files/LOS_EditCustomer_TestData.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MITech\Documents\TAF\automation-taf-project\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E976BCC-5F7C-43C0-AB86-6995A7028BFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39E78A15-7C7E-47BD-A51A-F7EEE63DDD85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2625" yWindow="3195" windowWidth="21600" windowHeight="12645" activeTab="3" xr2:uid="{B09B1DE0-549F-43F6-A9D1-0936A4CBD013}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="12645" activeTab="5" xr2:uid="{B09B1DE0-549F-43F6-A9D1-0936A4CBD013}"/>
   </bookViews>
   <sheets>
     <sheet name="CustInformation" sheetId="2" r:id="rId1"/>
     <sheet name="Credentials" sheetId="1" r:id="rId2"/>
     <sheet name="MainData" sheetId="3" r:id="rId3"/>
     <sheet name="Address" sheetId="4" r:id="rId4"/>
+    <sheet name="Family" sheetId="5" r:id="rId5"/>
+    <sheet name="JobData" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="200">
   <si>
     <t>ScenarioId</t>
   </si>
@@ -331,6 +333,303 @@
   </si>
   <si>
     <t>Edit Scenario Job Address</t>
+  </si>
+  <si>
+    <t>CustomerModel</t>
+  </si>
+  <si>
+    <t>FamilyName</t>
+  </si>
+  <si>
+    <t>IDType</t>
+  </si>
+  <si>
+    <t>IDNumber</t>
+  </si>
+  <si>
+    <t>IDExpiredDate</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>BirthPlace</t>
+  </si>
+  <si>
+    <t>BirthDate</t>
+  </si>
+  <si>
+    <t>NPWP</t>
+  </si>
+  <si>
+    <t>MotherMaidenName</t>
+  </si>
+  <si>
+    <t>CustomerRelationship</t>
+  </si>
+  <si>
+    <t>Professional</t>
+  </si>
+  <si>
+    <t>RANA</t>
+  </si>
+  <si>
+    <t>KTP</t>
+  </si>
+  <si>
+    <t>3603283107950001</t>
+  </si>
+  <si>
+    <t>12/12/2099</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>JAKARTA</t>
+  </si>
+  <si>
+    <t>12/12/1995</t>
+  </si>
+  <si>
+    <t>RINI</t>
+  </si>
+  <si>
+    <t>SELF</t>
+  </si>
+  <si>
+    <t>Employee</t>
+  </si>
+  <si>
+    <t>KITAP</t>
+  </si>
+  <si>
+    <t>3603283107950002</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>13/12/1995</t>
+  </si>
+  <si>
+    <t>RUNU</t>
+  </si>
+  <si>
+    <t>MOTHER</t>
+  </si>
+  <si>
+    <t>Small Medium Enterprise</t>
+  </si>
+  <si>
+    <t>KITAS</t>
+  </si>
+  <si>
+    <t>3603283107950003</t>
+  </si>
+  <si>
+    <t>BANDUNG</t>
+  </si>
+  <si>
+    <t>14/12/1995</t>
+  </si>
+  <si>
+    <t>RENE</t>
+  </si>
+  <si>
+    <t>SISTER</t>
+  </si>
+  <si>
+    <t>Non Professional</t>
+  </si>
+  <si>
+    <t>PASSPORT</t>
+  </si>
+  <si>
+    <t>3603283107950004</t>
+  </si>
+  <si>
+    <t>BEKASI</t>
+  </si>
+  <si>
+    <t>15/12/1995</t>
+  </si>
+  <si>
+    <t>BROTHER</t>
+  </si>
+  <si>
+    <t>ProfessionName</t>
+  </si>
+  <si>
+    <t>ProfessionalNo</t>
+  </si>
+  <si>
+    <t>JobPosition</t>
+  </si>
+  <si>
+    <t>JobStatus</t>
+  </si>
+  <si>
+    <t>InternalEmployee</t>
+  </si>
+  <si>
+    <t>IndustryTypeName</t>
+  </si>
+  <si>
+    <t>CompanyScale</t>
+  </si>
+  <si>
+    <t>InvestmentType</t>
+  </si>
+  <si>
+    <t>NumberofEmployee</t>
+  </si>
+  <si>
+    <t>EmploymentEstablishmentDateMonth</t>
+  </si>
+  <si>
+    <t>EmploymentEstablishmentDateYear</t>
+  </si>
+  <si>
+    <t>IsWellKnownCompany</t>
+  </si>
+  <si>
+    <t>PreviousCompanyName</t>
+  </si>
+  <si>
+    <t>PreviousEmployementDateMonth</t>
+  </si>
+  <si>
+    <t>PreviousEmployementDateYear</t>
+  </si>
+  <si>
+    <t>OtherBusinessName</t>
+  </si>
+  <si>
+    <t>OtherBussinessType</t>
+  </si>
+  <si>
+    <t>OtherJobPosition</t>
+  </si>
+  <si>
+    <t>OtherEmploymentEstablishmentDateMonth</t>
+  </si>
+  <si>
+    <t>OtherEmploymentEstablishmentDateYear</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>123214211</t>
+  </si>
+  <si>
+    <t>EXECUTIVE</t>
+  </si>
+  <si>
+    <t>PERMANENT</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>LARGE</t>
+  </si>
+  <si>
+    <t>Penanaman Modal Asing</t>
+  </si>
+  <si>
+    <t>wowow</t>
+  </si>
+  <si>
+    <t>1995</t>
+  </si>
+  <si>
+    <t>wewew</t>
+  </si>
+  <si>
+    <t>DIREKTUR</t>
+  </si>
+  <si>
+    <t>PT QA TEST2</t>
+  </si>
+  <si>
+    <t>SMALL</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>February</t>
+  </si>
+  <si>
+    <t>2001</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>1996</t>
+  </si>
+  <si>
+    <t>DIREKTUR UTAMA</t>
+  </si>
+  <si>
+    <t>PT QA TEST3</t>
+  </si>
+  <si>
+    <t>MEDIUM</t>
+  </si>
+  <si>
+    <t>Penanaman Modal Dalam Negeri</t>
+  </si>
+  <si>
+    <t>500</t>
+  </si>
+  <si>
+    <t>March</t>
+  </si>
+  <si>
+    <t>2002</t>
+  </si>
+  <si>
+    <t>1997</t>
+  </si>
+  <si>
+    <t>PEMBINA</t>
+  </si>
+  <si>
+    <t>PT QA TEST4</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>June</t>
+  </si>
+  <si>
+    <t>2003</t>
+  </si>
+  <si>
+    <t>1998</t>
+  </si>
+  <si>
+    <t>%JAKSA%</t>
+  </si>
+  <si>
+    <t>%PEMERINTAH%</t>
+  </si>
+  <si>
+    <t>Jaya Board</t>
+  </si>
+  <si>
+    <t>Milkyway</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>2012</t>
   </si>
 </sst>
 </file>
@@ -700,7 +999,7 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1036,7 +1335,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE6ABE60-5614-4142-A37F-7F588A409B68}">
   <dimension ref="A1:U4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="U5" sqref="U5"/>
     </sheetView>
   </sheetViews>
@@ -1253,4 +1552,540 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA44301B-7362-4DF4-8D97-A51219E0AAF8}">
+  <dimension ref="A1:L5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="G2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H2" t="s">
+        <v>118</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="K2" t="s">
+        <v>120</v>
+      </c>
+      <c r="L2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D3" t="s">
+        <v>123</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="G3" t="s">
+        <v>125</v>
+      </c>
+      <c r="H3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="K3" t="s">
+        <v>127</v>
+      </c>
+      <c r="L3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D4" t="s">
+        <v>130</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="G4" t="s">
+        <v>117</v>
+      </c>
+      <c r="H4" t="s">
+        <v>132</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="K4" t="s">
+        <v>134</v>
+      </c>
+      <c r="L4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C5" t="s">
+        <v>134</v>
+      </c>
+      <c r="D5" t="s">
+        <v>137</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="G5" t="s">
+        <v>125</v>
+      </c>
+      <c r="H5" t="s">
+        <v>139</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="K5" t="s">
+        <v>113</v>
+      </c>
+      <c r="L5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF542AAE-DC9C-4E13-90B2-6438DAE76B67}">
+  <dimension ref="A1:V5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="41" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="39" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" t="s">
+        <v>164</v>
+      </c>
+      <c r="E2" t="s">
+        <v>165</v>
+      </c>
+      <c r="G2" s="1"/>
+      <c r="H2" t="s">
+        <v>195</v>
+      </c>
+      <c r="I2" t="s">
+        <v>182</v>
+      </c>
+      <c r="J2" t="s">
+        <v>183</v>
+      </c>
+      <c r="K2" s="1"/>
+      <c r="L2" t="s">
+        <v>185</v>
+      </c>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" t="s">
+        <v>196</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="R2" t="s">
+        <v>197</v>
+      </c>
+      <c r="U2" t="s">
+        <v>198</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D3" t="s">
+        <v>172</v>
+      </c>
+      <c r="E3" t="s">
+        <v>165</v>
+      </c>
+      <c r="F3" t="s">
+        <v>173</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="H3" t="s">
+        <v>162</v>
+      </c>
+      <c r="I3" t="s">
+        <v>174</v>
+      </c>
+      <c r="J3" t="s">
+        <v>168</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="L3" t="s">
+        <v>176</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="O3" t="s">
+        <v>169</v>
+      </c>
+      <c r="P3" t="s">
+        <v>176</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="R3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D4" t="s">
+        <v>180</v>
+      </c>
+      <c r="E4" t="s">
+        <v>165</v>
+      </c>
+      <c r="F4" t="s">
+        <v>181</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="H4" t="s">
+        <v>162</v>
+      </c>
+      <c r="I4" t="s">
+        <v>182</v>
+      </c>
+      <c r="J4" t="s">
+        <v>183</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="L4" t="s">
+        <v>185</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="O4" t="s">
+        <v>169</v>
+      </c>
+      <c r="P4" t="s">
+        <v>185</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="R4" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D5" t="s">
+        <v>188</v>
+      </c>
+      <c r="E5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F5" t="s">
+        <v>189</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="H5" t="s">
+        <v>162</v>
+      </c>
+      <c r="I5" t="s">
+        <v>167</v>
+      </c>
+      <c r="J5" t="s">
+        <v>183</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="L5" t="s">
+        <v>191</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="O5" t="s">
+        <v>169</v>
+      </c>
+      <c r="P5" t="s">
+        <v>191</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="R5" t="s">
+        <v>171</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>